<commit_message>
Graficas no comparacion funcionando -- Actualizar .gitignore, Dockerfile y 25 más archivos...
</commit_message>
<xml_diff>
--- a/home/data/PMMA EXT_MACTAC_PAPEL RC.xlsx
+++ b/home/data/PMMA EXT_MACTAC_PAPEL RC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirey\Documents\DOCTORADO 17-18\CAPITULOS TESIS INDICE Y ANEXOS\CAPITULO VI\COLORIMETRÍA PARA GRÁFICAS ÁNGEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB155CF-C0D6-4F9B-ACDE-640FDAAE40C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B016E63-5302-4CF3-8CAA-641FEC986E77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6A44A0B7-9275-42A5-A797-CEA7C879B6AE}"/>
   </bookViews>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9522FB-A4EE-4158-958A-E59E8841E8F3}">
   <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N12" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4:AB30"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2465,11 +2465,11 @@
         <v>-0.94</v>
       </c>
       <c r="D26">
-        <v>-120.4</v>
+        <v>-12.4</v>
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>-121.34</v>
+        <v>-13.34</v>
       </c>
       <c r="K26">
         <v>51.07</v>
@@ -2494,15 +2494,15 @@
       </c>
       <c r="Q26">
         <f t="shared" si="5"/>
-        <v>-112.88000000000001</v>
+        <v>-4.8800000000000008</v>
       </c>
       <c r="R26">
         <f t="shared" si="6"/>
-        <v>115.19853905323627</v>
+        <v>23.507943338369696</v>
       </c>
       <c r="S26">
         <f t="shared" si="7"/>
-        <v>-129.27000000000001</v>
+        <v>-21.27</v>
       </c>
       <c r="U26">
         <v>57.92</v>
@@ -2527,15 +2527,15 @@
       </c>
       <c r="AA26">
         <f t="shared" si="2"/>
-        <v>-117.43</v>
+        <v>-9.43</v>
       </c>
       <c r="AB26">
         <f t="shared" si="9"/>
-        <v>119.98419812625329</v>
+        <v>26.369069001388731</v>
       </c>
       <c r="AC26">
         <f t="shared" si="10"/>
-        <v>-126.28</v>
+        <v>-18.28</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>